<commit_message>
Edit retro and time sheet
</commit_message>
<xml_diff>
--- a/Sprint 2/Time Sheet Sprint 2.xlsx
+++ b/Sprint 2/Time Sheet Sprint 2.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glynkendall\Desktop\2018 UNI\Semester 2\FIT2101\Full Project\my-awesome-project\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mad scientist\Desktop\my-awesome-project\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66F5855-67BD-4F9B-A976-532FC6581F28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9383487B-C104-44BE-8DBC-187A55EFE9AB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Michael</t>
   </si>
@@ -93,6 +86,9 @@
   </si>
   <si>
     <t>Looking over test cases</t>
+  </si>
+  <si>
+    <t>Editting files</t>
   </si>
 </sst>
 </file>
@@ -563,18 +559,18 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="86.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="86.54296875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.2">
+    <row r="1" spans="1:7" ht="12.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2" customHeight="1">
+    <row r="3" spans="1:7" ht="13.25" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -626,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.2">
+    <row r="5" spans="1:7" ht="12.5">
       <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
@@ -647,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.8">
+    <row r="6" spans="1:7" ht="14">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
@@ -668,7 +664,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.2">
+    <row r="7" spans="1:7" ht="12.5">
       <c r="A7" s="18" t="s">
         <v>2</v>
       </c>
@@ -686,10 +682,10 @@
       </c>
       <c r="G7">
         <f>SUMIF(A4:A29,"*Simon*",C4:C29)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="13.8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14">
       <c r="A8" s="18" t="s">
         <v>2</v>
       </c>
@@ -710,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.2">
+    <row r="9" spans="1:7" ht="12.5">
       <c r="A9" s="18" t="s">
         <v>2</v>
       </c>
@@ -724,7 +720,7 @@
         <v>43357</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.2">
+    <row r="10" spans="1:7" ht="12.5">
       <c r="A10" s="18" t="s">
         <v>2</v>
       </c>
@@ -738,7 +734,7 @@
         <v>43358</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.2">
+    <row r="11" spans="1:7" ht="12.5">
       <c r="A11" s="13" t="s">
         <v>0</v>
       </c>
@@ -752,7 +748,7 @@
         <v>43359</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.2">
+    <row r="12" spans="1:7" ht="12.5">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -766,7 +762,7 @@
         <v>43362</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.2">
+    <row r="13" spans="1:7" ht="12.5">
       <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
@@ -780,7 +776,7 @@
         <v>43362</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.2">
+    <row r="14" spans="1:7" ht="12.5">
       <c r="A14" s="15" t="s">
         <v>1</v>
       </c>
@@ -794,7 +790,7 @@
         <v>43362</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.2">
+    <row r="15" spans="1:7" ht="12.5">
       <c r="A15" s="15" t="s">
         <v>1</v>
       </c>
@@ -808,7 +804,7 @@
         <v>43363</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.2">
+    <row r="16" spans="1:7" ht="12.5">
       <c r="A16" s="15" t="s">
         <v>1</v>
       </c>
@@ -822,7 +818,7 @@
         <v>43364</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.2">
+    <row r="17" spans="1:4" ht="12.5">
       <c r="A17" s="9" t="s">
         <v>4</v>
       </c>
@@ -836,73 +832,81 @@
         <v>43364</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="13.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="1:4" ht="13.2">
+    <row r="18" spans="1:4" ht="12.5">
+      <c r="A18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>43362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12.5">
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="24"/>
     </row>
-    <row r="20" spans="1:4" ht="13.2">
+    <row r="20" spans="1:4" ht="12.5">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="26"/>
     </row>
-    <row r="21" spans="1:4" ht="13.2">
+    <row r="21" spans="1:4" ht="12.5">
       <c r="A21" s="25"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="1:4" ht="13.2">
+    <row r="22" spans="1:4" ht="12.5">
       <c r="A22" s="25"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
     </row>
-    <row r="23" spans="1:4" ht="13.2">
+    <row r="23" spans="1:4" ht="12.5">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="22"/>
     </row>
-    <row r="24" spans="1:4" ht="13.2">
+    <row r="24" spans="1:4" ht="12.5">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="1:4" ht="13.2">
+    <row r="25" spans="1:4" ht="12.5">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
     </row>
-    <row r="26" spans="1:4" ht="13.2">
+    <row r="26" spans="1:4" ht="12.5">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
     </row>
-    <row r="27" spans="1:4" ht="13.2">
+    <row r="27" spans="1:4" ht="12.5">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" ht="13.2">
+    <row r="28" spans="1:4" ht="12.5">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
     </row>
-    <row r="29" spans="1:4" ht="13.2">
+    <row r="29" spans="1:4" ht="12.5">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>

</xml_diff>